<commit_message>
fix sel card bug
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Value/CardValue.xlsx
+++ b/Assets/StreamingAssets/Value/CardValue.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\Value\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Downloads\UNR\CS 425\CS425-426\Assets\StreamingAssets\Value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FA4D2B-D0CF-4E37-8D11-AA5EAB83B002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDF6C80-5FD5-493F-8485-122D030BEF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>CardName</t>
   </si>
   <si>
-    <t>Rarity</t>
-  </si>
-  <si>
     <t>Ability</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>has slow speed. Damage is high. *unique ability: bullets have a chance to dismember enemies, causing them to do less damage to the player*</t>
+  </si>
+  <si>
+    <t>Rarity (0 = Common, 1 = Rare, 2 =VeryRare, 3 = Epic)</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,13 +417,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -432,16 +432,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -450,16 +450,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -468,16 +468,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -486,16 +486,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>